<commit_message>
221207 nvram(led status), interrupt(btn), timer(debounce) code
</commit_message>
<xml_diff>
--- a/cyw920706_ikh_221123.xlsx
+++ b/cyw920706_ikh_221123.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\CYPRESS\bt\cyw920706\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AF767D-0715-4552-B067-6E55C409FE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08612A1-5914-4622-BE79-439D082737CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="870" windowWidth="21450" windowHeight="13290" xr2:uid="{348F3D5B-D423-4BBA-AD3B-56CD4D9B69BC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{348F3D5B-D423-4BBA-AD3B-56CD4D9B69BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -1087,7 +1087,7 @@
 공용 풀은 애플리케이션의 wiceed_bt_cfg_buf_pool_t를 사용하여 지정해야 한다</t>
       </text>
     </comment>
-    <comment ref="I28" authorId="0" shapeId="0" xr:uid="{D052F00E-C02D-49DA-AA48-3161E10244B2}">
+    <comment ref="I29" authorId="0" shapeId="0" xr:uid="{D052F00E-C02D-49DA-AA48-3161E10244B2}">
       <text>
         <r>
           <rPr>
@@ -1102,7 +1102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K28" authorId="10" shapeId="0" xr:uid="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
+    <comment ref="K29" authorId="10" shapeId="0" xr:uid="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1111,7 +1111,7 @@
 우리는 서비스 연결을 만들 때 동일한 것을 사용해야 합니다.</t>
       </text>
     </comment>
-    <comment ref="K29" authorId="0" shapeId="0" xr:uid="{BE0CD214-DBEC-47D2-8442-B6DC742700F8}">
+    <comment ref="K30" authorId="0" shapeId="0" xr:uid="{BE0CD214-DBEC-47D2-8442-B6DC742700F8}">
       <text>
         <r>
           <rPr>
@@ -1199,7 +1199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M29" authorId="0" shapeId="0" xr:uid="{97409CBB-F809-494F-BC12-29F09AFB78B6}">
+    <comment ref="M30" authorId="0" shapeId="0" xr:uid="{97409CBB-F809-494F-BC12-29F09AFB78B6}">
       <text>
         <r>
           <rPr>
@@ -1287,7 +1287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M30" authorId="11" shapeId="0" xr:uid="{A2079DE1-B458-45FD-A842-91298A20C566}">
+    <comment ref="M31" authorId="11" shapeId="0" xr:uid="{A2079DE1-B458-45FD-A842-91298A20C566}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1299,7 +1299,7 @@
 서버의 경우 클라이언트가 (scn * 2 + 1) dlci를 사용하여 호출할 경우 나중에 DLCI를 변경할 수 있습니다.</t>
       </text>
     </comment>
-    <comment ref="O30" authorId="0" shapeId="0" xr:uid="{4611D336-9E6D-4C22-B5FE-D32DADAFF458}">
+    <comment ref="O31" authorId="0" shapeId="0" xr:uid="{4611D336-9E6D-4C22-B5FE-D32DADAFF458}">
       <text>
         <r>
           <rPr>
@@ -1313,7 +1313,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O32" authorId="0" shapeId="0" xr:uid="{56C4381F-0E2D-4DC1-B651-95FF79BFC877}">
+    <comment ref="O33" authorId="0" shapeId="0" xr:uid="{56C4381F-0E2D-4DC1-B651-95FF79BFC877}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{6510170B-43BC-4846-A24D-A3E5B452097B}">
+    <comment ref="I34" authorId="0" shapeId="0" xr:uid="{6510170B-43BC-4846-A24D-A3E5B452097B}">
       <text>
         <r>
           <rPr>
@@ -1405,7 +1405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O33" authorId="0" shapeId="0" xr:uid="{317D5308-F94D-4114-9626-A1ABA61F3777}">
+    <comment ref="O34" authorId="0" shapeId="0" xr:uid="{317D5308-F94D-4114-9626-A1ABA61F3777}">
       <text>
         <r>
           <rPr>
@@ -1535,7 +1535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I34" authorId="12" shapeId="0" xr:uid="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
+    <comment ref="I35" authorId="12" shapeId="0" xr:uid="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1547,7 +1547,7 @@
 @param[in]       interval</t>
       </text>
     </comment>
-    <comment ref="O34" authorId="0" shapeId="0" xr:uid="{9B2EBD72-524E-4ABF-9500-856F3D979BA8}">
+    <comment ref="O35" authorId="0" shapeId="0" xr:uid="{9B2EBD72-524E-4ABF-9500-856F3D979BA8}">
       <text>
         <r>
           <rPr>
@@ -1561,7 +1561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q34" authorId="0" shapeId="0" xr:uid="{C345AC06-B5E7-4A44-8754-5790C3BB3E5A}">
+    <comment ref="Q35" authorId="0" shapeId="0" xr:uid="{C345AC06-B5E7-4A44-8754-5790C3BB3E5A}">
       <text>
         <r>
           <rPr>
@@ -1575,7 +1575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O35" authorId="0" shapeId="0" xr:uid="{F33E7AA5-0B4C-4C82-B80D-5F15A2B41293}">
+    <comment ref="O36" authorId="0" shapeId="0" xr:uid="{F33E7AA5-0B4C-4C82-B80D-5F15A2B41293}">
       <text>
         <r>
           <rPr>
@@ -1589,7 +1589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{A990AD82-4358-4EBE-8FC5-92F23A70B0A2}">
+    <comment ref="I39" authorId="0" shapeId="0" xr:uid="{A990AD82-4358-4EBE-8FC5-92F23A70B0A2}">
       <text>
         <r>
           <rPr>
@@ -1699,7 +1699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="0" shapeId="0" xr:uid="{F5CF7399-0971-453D-8DD9-FFE822A63A0A}">
+    <comment ref="K39" authorId="0" shapeId="0" xr:uid="{F5CF7399-0971-453D-8DD9-FFE822A63A0A}">
       <text>
         <r>
           <rPr>
@@ -1850,7 +1850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G39" authorId="13" shapeId="0" xr:uid="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
+    <comment ref="G40" authorId="13" shapeId="0" xr:uid="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
       <text>
         <t xml:space="preserve">[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1861,7 +1861,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="I39" authorId="0" shapeId="0" xr:uid="{FC06FE87-1FC8-4894-945B-F8DED4ED8CA8}">
+    <comment ref="I40" authorId="0" shapeId="0" xr:uid="{FC06FE87-1FC8-4894-945B-F8DED4ED8CA8}">
       <text>
         <r>
           <rPr>
@@ -1889,7 +1889,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E42" authorId="14" shapeId="0" xr:uid="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
+    <comment ref="E43" authorId="14" shapeId="0" xr:uid="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1898,7 +1898,7 @@
 전달된 버퍼를 리턴한다</t>
       </text>
     </comment>
-    <comment ref="K42" authorId="0" shapeId="0" xr:uid="{7D551CA2-F55A-4A6E-8323-7E1A7EBF28C6}">
+    <comment ref="K43" authorId="0" shapeId="0" xr:uid="{7D551CA2-F55A-4A6E-8323-7E1A7EBF28C6}">
       <text>
         <r>
           <rPr>
@@ -1956,7 +1956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="0" shapeId="0" xr:uid="{5B1C2D12-1336-4608-8520-7E6A74492A31}">
+    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{5B1C2D12-1336-4608-8520-7E6A74492A31}">
       <text>
         <r>
           <rPr>
@@ -2017,7 +2017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K43" authorId="15" shapeId="0" xr:uid="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
+    <comment ref="K44" authorId="15" shapeId="0" xr:uid="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2025,7 +2025,7 @@
     전송을 통해 hci 추적 데이터를 보내는 함수</t>
       </text>
     </comment>
-    <comment ref="I46" authorId="16" shapeId="0" xr:uid="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
+    <comment ref="I47" authorId="16" shapeId="0" xr:uid="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2033,7 +2033,7 @@
     GPIO 드라이버 초기화 함수</t>
       </text>
     </comment>
-    <comment ref="I47" authorId="0" shapeId="0" xr:uid="{C18FEF3D-1B3F-41B0-91DD-684F4C00BA73}">
+    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{C18FEF3D-1B3F-41B0-91DD-684F4C00BA73}">
       <text>
         <r>
           <rPr>
@@ -2101,7 +2101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K50" authorId="17" shapeId="0" xr:uid="{6EA8C629-9993-46C6-A087-93837636CB40}">
+    <comment ref="K51" authorId="17" shapeId="0" xr:uid="{6EA8C629-9993-46C6-A087-93837636CB40}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2109,7 +2109,7 @@
     가능한 많은 데이터를 보내는 테스트 함수</t>
       </text>
     </comment>
-    <comment ref="M50" authorId="18" shapeId="0" xr:uid="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
+    <comment ref="M51" authorId="18" shapeId="0" xr:uid="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2117,7 +2117,7 @@
     가능한 많은 데이터를 보내는 테스트 함수</t>
       </text>
     </comment>
-    <comment ref="M51" authorId="19" shapeId="0" xr:uid="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
+    <comment ref="M52" authorId="19" shapeId="0" xr:uid="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2126,7 +2126,7 @@
 없으면 False</t>
       </text>
     </comment>
-    <comment ref="I58" authorId="20" shapeId="0" xr:uid="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
+    <comment ref="I59" authorId="20" shapeId="0" xr:uid="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
       <text>
         <t xml:space="preserve">[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2137,7 +2137,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="K60" authorId="21" shapeId="0" xr:uid="{97AD7065-CF38-4472-BC49-676025D10EB8}">
+    <comment ref="K61" authorId="21" shapeId="0" xr:uid="{97AD7065-CF38-4472-BC49-676025D10EB8}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2152,7 +2152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="290">
   <si>
     <t>wiced_hal_puart_init()</t>
   </si>
@@ -2732,10 +2732,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>wiced_bt_set_pairable_mode()</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>spp_rfcomm_start_server</t>
   </si>
   <si>
@@ -2803,10 +2799,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>wiced_bt_rfcomm_init()</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>#ifdef HCI_TRACE_OVER_TRANSPORT</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2824,10 +2816,6 @@
   </si>
   <si>
     <t>wiced_hal_gpio_get_pin_interrupt_status()</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>wiced_bt_spp_startup()        //* @param[in] : &amp;spp_reg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -3417,6 +3405,22 @@
   </si>
   <si>
     <t>/* Initialize Stack and Register Management Callback */</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">wiced_bt_spp_startup(&amp;spp_reg)       </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPP library 초기화하고, RFCOMM 서비스를 시작하는 함수</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wiced_bt_rfcomm_init()</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">RFCOMM에서 사용될 private pool를 할당하는 함수 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4297,7 +4301,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>1830294</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="184731" cy="264560"/>
@@ -4458,13 +4462,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1372764</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>59764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>5245353</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>183590</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4837,57 +4841,57 @@
     <text>공용 풀에서 버퍼를 할당하는 함수
 공용 풀은 애플리케이션의 wiceed_bt_cfg_buf_pool_t를 사용하여 지정해야 한다</text>
   </threadedComment>
-  <threadedComment ref="K28" dT="2022-11-24T04:27:40.26" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
+  <threadedComment ref="K29" dT="2022-11-24T04:27:40.26" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
     <text>응용 프로그램은 SDP 레코드를 만드는 데 사용한 scn을 전달합니다.  
 우리는 서비스 연결을 만들 때 동일한 것을 사용해야 합니다.</text>
   </threadedComment>
-  <threadedComment ref="M30" dT="2022-11-24T02:00:51.90" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{A2079DE1-B458-45FD-A842-91298A20C566}">
+  <threadedComment ref="M31" dT="2022-11-24T02:00:51.90" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{A2079DE1-B458-45FD-A842-91298A20C566}">
     <text>피어 장치에 대한 직렬 포트 연결을 설정하거나 RFCOMM이 피어 장치의 연결을 수락하도록 허용합니다.
 서버가 여러 개의 동시 연결을 허용할 준비가 된 경우 서버는 동일한 scn 매개 변수를 사용하여 이 함수를 여러 번 호출할 수 있습니다.
 클라이언트가 기존의 none 이니시에이터 멀티플렉서 채널에서 연결을 시작하는 경우 연결의 DLCI는 (scn * 2 + 1)입니다.  
 그렇지 않으면 (scn * 2)입니다. 
 서버의 경우 클라이언트가 (scn * 2 + 1) dlci를 사용하여 호출할 경우 나중에 DLCI를 변경할 수 있습니다.</text>
   </threadedComment>
-  <threadedComment ref="I34" dT="2022-11-24T00:41:57.09" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
+  <threadedComment ref="I35" dT="2022-11-24T00:41:57.09" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
     <text>Set discoverability(검색가능성 설정 함수)
 Duration이 interval보다 작거나 같아야 한다.
 @param[in]       inq_mode
 @param[in]       duration 
 @param[in]       interval</text>
   </threadedComment>
-  <threadedComment ref="G39" dT="2022-12-02T04:49:13.01" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
+  <threadedComment ref="G40" dT="2022-12-02T04:49:13.01" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
     <text xml:space="preserve">NVRAM에 데이터를 쓰는 함수
 APP에 최대 255byte까지 쓸 수 있다(vs id 섹션 1개당)
 랑크키를 동일한 NVRAM ID에다 저장하여 이전 페어링에 덮어쓸 수 있습니다(있는 경우).
 </text>
   </threadedComment>
-  <threadedComment ref="E42" dT="2022-11-23T07:02:06.50" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
+  <threadedComment ref="E43" dT="2022-11-23T07:02:06.50" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
     <text>NVRAM으로부터 데이터를 읽는 함수,
 전달된 버퍼를 리턴한다</text>
   </threadedComment>
-  <threadedComment ref="K43" dT="2022-11-23T06:43:22.83" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
+  <threadedComment ref="K44" dT="2022-11-23T06:43:22.83" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
     <text>전송을 통해 hci 추적 데이터를 보내는 함수</text>
   </threadedComment>
-  <threadedComment ref="I46" dT="2022-11-25T00:25:47.65" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
+  <threadedComment ref="I47" dT="2022-11-25T00:25:47.65" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
     <text>GPIO 드라이버 초기화 함수</text>
   </threadedComment>
-  <threadedComment ref="K50" dT="2022-11-29T03:40:28.85" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6EA8C629-9993-46C6-A087-93837636CB40}">
+  <threadedComment ref="K51" dT="2022-11-29T03:40:28.85" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{6EA8C629-9993-46C6-A087-93837636CB40}">
     <text>가능한 많은 데이터를 보내는 테스트 함수</text>
   </threadedComment>
-  <threadedComment ref="M50" dT="2022-11-29T03:40:28.85" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
+  <threadedComment ref="M51" dT="2022-11-29T03:40:28.85" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
     <text>가능한 많은 데이터를 보내는 테스트 함수</text>
   </threadedComment>
-  <threadedComment ref="M51" dT="2022-12-01T02:30:49.80" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
+  <threadedComment ref="M52" dT="2022-12-01T02:30:49.80" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
     <text>Queue에 데이터를 전달 할 수 있으면 Ture,
 없으면 False</text>
   </threadedComment>
-  <threadedComment ref="I58" dT="2022-11-25T00:45:20.83" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
+  <threadedComment ref="I59" dT="2022-11-25T00:45:20.83" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
     <text xml:space="preserve">지정한 핀의 현재 구성을 검색합니다.
 위의 핀 구성 세트를 가져옵니다.
 모든 입력 매개 변수 값이 범위 내에 있어야 합니다. 그렇지 않으면 기능이 작동하지 않습니다.
 </text>
   </threadedComment>
-  <threadedComment ref="K60" dT="2022-11-25T01:05:20.13" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{97AD7065-CF38-4472-BC49-676025D10EB8}">
+  <threadedComment ref="K61" dT="2022-11-25T01:05:20.13" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{97AD7065-CF38-4472-BC49-676025D10EB8}">
     <text>타이머를 시작하기 전에 타이머를 초기화해야 합니다. 
 타이머를 실행하면 칩의 저전력 모드를 방해합니다. 
 저전력 모드를 유지하는 시간은 실행 중인 타이머의 시간 초과 값에 따라 달라집니다. 즉, 절전 시간은 활성 타이머 중 다음 타이머가 만료되는 시간에 따라 달라집니다.</text>
@@ -4897,10 +4901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CD9804-2490-4F6A-966A-5BB5914DA299}">
-  <dimension ref="B2:Q71"/>
+  <dimension ref="B2:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C21"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4955,7 +4959,7 @@
         <v>99</v>
       </c>
       <c r="M5" s="75" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
@@ -4972,7 +4976,7 @@
         <v>101</v>
       </c>
       <c r="M6" s="28" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -4989,7 +4993,7 @@
         <v>103</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5006,18 +5010,18 @@
         <v>104</v>
       </c>
       <c r="M8" s="75" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="68.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="71" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>59</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5025,13 +5029,13 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M10" s="28" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="O10" s="75" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5043,12 +5047,12 @@
       </c>
       <c r="M11" s="28"/>
       <c r="O11" s="29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E12" s="57" t="s">
         <v>64</v>
@@ -5057,7 +5061,7 @@
         <v>64</v>
       </c>
       <c r="M12" s="28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5072,7 +5076,7 @@
       </c>
       <c r="M13" s="29"/>
       <c r="O13" s="75" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5084,7 +5088,7 @@
         <v>75</v>
       </c>
       <c r="O14" s="28" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5099,7 +5103,7 @@
         <v>84</v>
       </c>
       <c r="O15" s="28" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.45">
@@ -5129,7 +5133,7 @@
         <v>80</v>
       </c>
       <c r="O17" s="28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.45">
@@ -5140,13 +5144,13 @@
         <v>70</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K18" s="38" t="s">
         <v>81</v>
       </c>
       <c r="O18" s="28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5156,13 +5160,13 @@
         <v>71</v>
       </c>
       <c r="G19" s="76" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="K19" s="38" t="s">
         <v>82</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -5207,7 +5211,7 @@
       <c r="B24" s="3"/>
       <c r="D24" s="36"/>
       <c r="I24" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>57</v>
@@ -5217,17 +5221,17 @@
       <c r="B25" s="3"/>
       <c r="D25" s="36"/>
       <c r="E25" s="71" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="I25" s="28"/>
       <c r="K25" s="29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B26" s="3"/>
       <c r="C26" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D26" s="36"/>
       <c r="I26" s="28"/>
@@ -5235,392 +5239,403 @@
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C27" t="s">
-        <v>274</v>
-      </c>
-      <c r="G27" s="33" t="s">
-        <v>66</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="D27" s="36"/>
       <c r="I27" s="28" t="s">
-        <v>129</v>
+        <v>288</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C28" t="s">
-        <v>275</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I28" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="K28" s="32" t="s">
-        <v>111</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C29" t="s">
-        <v>276</v>
-      </c>
-      <c r="I29" s="28"/>
-      <c r="K29" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="M29" s="31" t="s">
-        <v>112</v>
+        <v>272</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="57" t="s">
+        <v>286</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C30" t="s">
-        <v>277</v>
-      </c>
-      <c r="G30" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C31" t="s">
+        <v>274</v>
+      </c>
+      <c r="G31" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="28"/>
-      <c r="M30" s="29" t="s">
+      <c r="I31" s="28"/>
+      <c r="M31" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="O31" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="O30" s="31" t="s">
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="G32" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="I32" s="35"/>
+      <c r="O32" s="28" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="G31" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" s="35"/>
-      <c r="O31" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C32" t="s">
-        <v>273</v>
-      </c>
-      <c r="E32" s="43"/>
-      <c r="G32" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="O32" s="28" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="33" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C33" t="s">
-        <v>278</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>88</v>
+        <v>270</v>
+      </c>
+      <c r="E33" s="43"/>
+      <c r="G33" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="I33" s="28" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="O33" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q33" s="30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C34" t="s">
-        <v>279</v>
+        <v>275</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>88</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="O34" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q34" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I35" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="O35" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q35" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C36" t="s">
+        <v>274</v>
+      </c>
+      <c r="I36" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O35" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q35" s="29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.45">
-      <c r="I36" s="28"/>
-    </row>
-    <row r="37" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C37" t="s">
-        <v>273</v>
-      </c>
-      <c r="I37" s="42" t="s">
-        <v>124</v>
-      </c>
+      <c r="O36" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q36" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="I37" s="28"/>
     </row>
     <row r="38" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C38" t="s">
-        <v>280</v>
-      </c>
-      <c r="G38" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I38" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="K38" s="32" t="s">
-        <v>21</v>
+        <v>270</v>
+      </c>
+      <c r="I38" s="42" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C39" t="s">
-        <v>281</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="I39" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="K39" s="29" t="s">
-        <v>23</v>
+        <v>277</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="K39" s="32" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C40" t="s">
-        <v>277</v>
-      </c>
-      <c r="I40" s="28"/>
+        <v>278</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K40" s="29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="41" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G41" s="31" t="s">
+      <c r="C41" t="s">
+        <v>274</v>
+      </c>
+      <c r="I41" s="28"/>
+    </row>
+    <row r="42" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G42" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="42" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C42" t="s">
-        <v>273</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I42" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="K42" s="32" t="s">
-        <v>85</v>
+      <c r="I42" s="42" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C43" t="s">
-        <v>282</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="I43" s="28"/>
-      <c r="K43" s="28" t="s">
-        <v>83</v>
+        <v>270</v>
+      </c>
+      <c r="E43" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C44" t="s">
-        <v>283</v>
+        <v>279</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="I44" s="28"/>
-      <c r="K44" s="29"/>
-    </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="K44" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C45" t="s">
-        <v>277</v>
-      </c>
-      <c r="I45" s="42" t="s">
-        <v>131</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="K45" s="29"/>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.45">
-      <c r="I46" s="65" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C47" t="s">
-        <v>273</v>
-      </c>
+      <c r="C46" t="s">
+        <v>274</v>
+      </c>
+      <c r="I46" s="42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I47" s="65" t="s">
-        <v>211</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C48" t="s">
-        <v>284</v>
-      </c>
-      <c r="G48" t="s">
-        <v>123</v>
+        <v>270</v>
       </c>
       <c r="I48" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="K48" s="32" t="s">
-        <v>133</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C49" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G49" t="s">
         <v>122</v>
       </c>
-      <c r="I49" s="28"/>
-      <c r="K49" s="28" t="s">
-        <v>134</v>
+      <c r="I49" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="K49" s="32" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C50" t="s">
-        <v>277</v>
-      </c>
-      <c r="I50" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="K50" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="G50" t="s">
+        <v>121</v>
+      </c>
+      <c r="I50" s="28"/>
+      <c r="K50" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C51" t="s">
+        <v>274</v>
+      </c>
+      <c r="I51" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K51" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="M50" s="55" t="s">
+      <c r="M51" s="55" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="M51" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="53" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="54" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I54" s="55" t="s">
-        <v>215</v>
-      </c>
-    </row>
+    <row r="52" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M52" s="30" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="54" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="55" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G55" t="s">
-        <v>219</v>
-      </c>
-      <c r="I55" s="64" t="s">
+      <c r="I55" s="55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G56" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="56" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I56" s="65" t="s">
+      <c r="I56" s="64" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I57" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="K57" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="I58" s="28"/>
+      <c r="K58" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I59" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="K59" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="K56" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="I57" s="28"/>
-      <c r="K57" s="27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I58" s="66" t="s">
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="K60" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="K58" s="28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="K59" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="M59" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="K60" s="65" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="61" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="K61" s="29"/>
-    </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="I62" t="s">
-        <v>218</v>
-      </c>
+      <c r="M60" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="K61" s="65" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K62" s="29"/>
     </row>
     <row r="63" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I63" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="I64" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="9:13" x14ac:dyDescent="0.45">
+      <c r="K65" t="s">
+        <v>220</v>
+      </c>
+      <c r="M65" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="64" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="K64" t="s">
-        <v>223</v>
-      </c>
-      <c r="M64" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="66" spans="9:13" x14ac:dyDescent="0.45">
-      <c r="I66" t="s">
-        <v>225</v>
-      </c>
-      <c r="M66" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="67" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="68" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I68" s="55" t="s">
+    <row r="67" spans="9:13" x14ac:dyDescent="0.45">
+      <c r="I67" t="s">
+        <v>222</v>
+      </c>
+      <c r="M67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="69" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I69" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="M69" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I70" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I71" s="53" t="s">
+        <v>250</v>
+      </c>
+      <c r="K71" s="70" t="s">
         <v>251</v>
       </c>
-      <c r="M68" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="69" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I69" s="28" t="s">
+      <c r="M71" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I72" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="K72" s="30" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="70" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I70" s="53" t="s">
-        <v>253</v>
-      </c>
-      <c r="K70" s="70" t="s">
-        <v>254</v>
-      </c>
-      <c r="M70" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="71" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I71" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="K71" s="30" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -6177,7 +6192,7 @@
     <row r="1" spans="2:25" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B2" s="44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
@@ -6205,7 +6220,7 @@
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B3" s="47" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="48"/>
@@ -6233,7 +6248,7 @@
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B4" s="47" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -6261,7 +6276,7 @@
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B5" s="47" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -6289,7 +6304,7 @@
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B6" s="47" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
@@ -6343,7 +6358,7 @@
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B8" s="47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -6371,7 +6386,7 @@
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B9" s="47" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
@@ -6399,7 +6414,7 @@
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B10" s="47" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C10" s="48"/>
       <c r="D10" s="48"/>
@@ -6427,7 +6442,7 @@
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B11" s="47" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C11" s="48"/>
       <c r="D11" s="48"/>
@@ -6455,7 +6470,7 @@
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B12" s="47" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C12" s="48"/>
       <c r="D12" s="48"/>
@@ -6483,7 +6498,7 @@
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B13" s="47" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
@@ -6511,7 +6526,7 @@
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B14" s="47" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="48"/>
@@ -6539,7 +6554,7 @@
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B15" s="47" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="48"/>
@@ -6567,7 +6582,7 @@
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B16" s="47" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C16" s="48"/>
       <c r="D16" s="48"/>
@@ -6595,7 +6610,7 @@
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B17" s="47" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C17" s="48"/>
       <c r="D17" s="48"/>
@@ -6623,7 +6638,7 @@
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B18" s="47" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="48"/>
@@ -6651,7 +6666,7 @@
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B19" s="47" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C19" s="48"/>
       <c r="D19" s="48"/>
@@ -6679,7 +6694,7 @@
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B20" s="47" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
@@ -6707,7 +6722,7 @@
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B21" s="47" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C21" s="48"/>
       <c r="D21" s="48"/>
@@ -6761,7 +6776,7 @@
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B23" s="47" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
@@ -6789,7 +6804,7 @@
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B24" s="47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
@@ -6817,7 +6832,7 @@
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B25" s="47" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C25" s="48"/>
       <c r="D25" s="48"/>
@@ -6845,7 +6860,7 @@
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B26" s="47" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C26" s="48"/>
       <c r="D26" s="48"/>
@@ -6899,7 +6914,7 @@
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B28" s="47" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
@@ -6927,7 +6942,7 @@
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B29" s="47" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
@@ -6981,7 +6996,7 @@
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B31" s="47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
@@ -7009,7 +7024,7 @@
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B32" s="47" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
@@ -7063,7 +7078,7 @@
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B34" s="47" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
@@ -7091,7 +7106,7 @@
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B35" s="47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
@@ -7119,7 +7134,7 @@
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B36" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C36" s="48"/>
       <c r="D36" s="48"/>
@@ -7147,7 +7162,7 @@
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B37" s="47" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C37" s="48"/>
       <c r="D37" s="48"/>
@@ -7201,7 +7216,7 @@
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B39" s="47" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C39" s="48"/>
       <c r="D39" s="48"/>
@@ -7229,7 +7244,7 @@
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B40" s="47" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C40" s="48"/>
       <c r="D40" s="48"/>
@@ -7257,7 +7272,7 @@
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B41" s="47" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C41" s="48"/>
       <c r="D41" s="48"/>
@@ -7285,7 +7300,7 @@
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B42" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C42" s="48"/>
       <c r="D42" s="48"/>
@@ -7313,7 +7328,7 @@
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B43" s="47" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C43" s="48"/>
       <c r="D43" s="48"/>
@@ -7341,7 +7356,7 @@
     </row>
     <row r="44" spans="2:25" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B44" s="50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C44" s="51"/>
       <c r="D44" s="51"/>
@@ -7391,12 +7406,12 @@
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L3" s="68" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B4" s="67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C4" s="67"/>
       <c r="D4" s="67"/>
@@ -7407,7 +7422,7 @@
       <c r="I4" s="67"/>
       <c r="J4" s="67"/>
       <c r="L4" s="68" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
@@ -7428,7 +7443,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B6" s="67" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="67"/>
       <c r="D6" s="67"/>
@@ -7439,12 +7454,12 @@
       <c r="I6" s="67"/>
       <c r="J6" s="67"/>
       <c r="L6" s="68" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="67" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C7" s="67"/>
       <c r="D7" s="67"/>
@@ -7455,12 +7470,12 @@
       <c r="I7" s="67"/>
       <c r="J7" s="67"/>
       <c r="L7" s="68" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="67" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C8" s="67"/>
       <c r="D8" s="67"/>
@@ -7471,12 +7486,12 @@
       <c r="I8" s="67"/>
       <c r="J8" s="67"/>
       <c r="L8" s="68" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" s="67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C9" s="67"/>
       <c r="D9" s="67"/>
@@ -7487,12 +7502,12 @@
       <c r="I9" s="67"/>
       <c r="J9" s="67"/>
       <c r="L9" s="68" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" s="67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C10" s="67"/>
       <c r="D10" s="67"/>
@@ -7506,7 +7521,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B11" s="67" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C11" s="67"/>
       <c r="D11" s="67"/>
@@ -7517,12 +7532,12 @@
       <c r="I11" s="67"/>
       <c r="J11" s="67"/>
       <c r="L11" s="68" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" s="67" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
@@ -7533,12 +7548,12 @@
       <c r="I12" s="67"/>
       <c r="J12" s="67"/>
       <c r="L12" s="68" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B13" s="67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C13" s="67"/>
       <c r="D13" s="67"/>
@@ -7549,7 +7564,7 @@
       <c r="I13" s="67"/>
       <c r="J13" s="67"/>
       <c r="L13" s="68" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
@@ -7563,7 +7578,7 @@
       <c r="I14" s="67"/>
       <c r="J14" s="67"/>
       <c r="L14" s="68" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
@@ -7580,7 +7595,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B16" s="67" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C16" s="67"/>
       <c r="D16" s="67"/>
@@ -7591,12 +7606,12 @@
       <c r="I16" s="67"/>
       <c r="J16" s="67"/>
       <c r="L16" s="68" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B17" s="67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C17" s="67"/>
       <c r="D17" s="67"/>
@@ -7607,7 +7622,7 @@
       <c r="I17" s="67"/>
       <c r="J17" s="67"/>
       <c r="L17" s="68" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
@@ -7626,7 +7641,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B19" s="67" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C19" s="67"/>
       <c r="D19" s="67"/>
@@ -7637,12 +7652,12 @@
       <c r="I19" s="67"/>
       <c r="J19" s="67"/>
       <c r="L19" s="68" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B20" s="67" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C20" s="67"/>
       <c r="D20" s="67"/>
@@ -7653,12 +7668,12 @@
       <c r="I20" s="67"/>
       <c r="J20" s="67"/>
       <c r="L20" s="68" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B21" s="67" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C21" s="67"/>
       <c r="D21" s="67"/>
@@ -7672,7 +7687,7 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B22" s="67" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C22" s="67"/>
       <c r="D22" s="67"/>
@@ -7683,12 +7698,12 @@
       <c r="I22" s="67"/>
       <c r="J22" s="67"/>
       <c r="L22" s="68" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B23" s="67" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C23" s="67"/>
       <c r="D23" s="67"/>
@@ -7699,12 +7714,12 @@
       <c r="I23" s="67"/>
       <c r="J23" s="67"/>
       <c r="L23" s="68" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B24" s="67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C24" s="67"/>
       <c r="D24" s="67"/>
@@ -7718,7 +7733,7 @@
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B25" s="67" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C25" s="67"/>
       <c r="D25" s="67"/>
@@ -7729,12 +7744,12 @@
       <c r="I25" s="67"/>
       <c r="J25" s="67"/>
       <c r="L25" s="68" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L26" s="68" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
@@ -7742,12 +7757,12 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L28" s="68" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L29" s="68" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.45">
@@ -7755,27 +7770,27 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L31" s="68" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L32" s="68" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L33" s="68" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L34" s="68" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L35" s="68" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7799,13 +7814,13 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="68" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" s="68" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.45">
@@ -7813,12 +7828,12 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="68" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="69" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.45">
@@ -7828,7 +7843,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="68" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
@@ -7836,27 +7851,27 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="68" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" s="68" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="68" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="68" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="68" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
@@ -7867,17 +7882,17 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" s="68" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="68" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
@@ -7891,12 +7906,12 @@
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" s="68" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" s="68" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
@@ -7907,27 +7922,27 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" s="68" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" s="68" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" s="68" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" s="68" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" s="68" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify short&long key press, change func name
</commit_message>
<xml_diff>
--- a/cyw920706_ikh_221123.xlsx
+++ b/cyw920706_ikh_221123.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\CYPRESS\bt\cyw920706\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312F6115-85EF-4C43-8F61-32AA1554D369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF1C26F-F117-442F-9EAE-AF9B7AFCA9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{348F3D5B-D423-4BBA-AD3B-56CD4D9B69BC}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="25760" windowHeight="15440" xr2:uid="{348F3D5B-D423-4BBA-AD3B-56CD4D9B69BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -49,6 +49,8 @@
     <author>tc={86E313D0-4B3E-4C94-8368-FCB9021D3AC7}</author>
     <author>tc={440AAFC9-9208-4331-97A1-DCEDF99B63EA}</author>
     <author>tc={C9FB7DAD-5DDC-4399-8A44-DEF628271C75}</author>
+    <author>tc={B44307AE-C7C2-42B1-B54E-E1BA9BFD21B7}</author>
+    <author>tc={FCC7E135-E087-4D67-9EA3-671A48F4D91D}</author>
     <author>tc={C78B3C0A-6A2B-411F-BC5C-56658A712951}</author>
     <author>tc={F531306B-CB68-4718-8EE2-9B39CCD8B1AB}</author>
     <author>tc={08D18B8D-AB5A-4272-8E49-9E16A59F835D}</author>
@@ -888,7 +890,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="K18" authorId="7" shapeId="0" xr:uid="{C78B3C0A-6A2B-411F-BC5C-56658A712951}">
+    <comment ref="K16" authorId="7" shapeId="0" xr:uid="{B44307AE-C7C2-42B1-B54E-E1BA9BFD21B7}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    Check to see if there is any data ready in the RX FIFO.</t>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="8" shapeId="0" xr:uid="{FCC7E135-E087-4D67-9EA3-671A48F4D91D}">
+      <text>
+        <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+    Read one byte via the RX line.</t>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="9" shapeId="0" xr:uid="{C78B3C0A-6A2B-411F-BC5C-56658A712951}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -896,7 +914,7 @@
     바이트 집합을 순차적으로 쓰는 함수</t>
       </text>
     </comment>
-    <comment ref="K19" authorId="8" shapeId="0" xr:uid="{F531306B-CB68-4718-8EE2-9B39CCD8B1AB}">
+    <comment ref="K19" authorId="10" shapeId="0" xr:uid="{F531306B-CB68-4718-8EE2-9B39CCD8B1AB}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1078,7 +1096,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K25" authorId="9" shapeId="0" xr:uid="{08D18B8D-AB5A-4272-8E49-9E16A59F835D}">
+    <comment ref="K25" authorId="11" shapeId="0" xr:uid="{08D18B8D-AB5A-4272-8E49-9E16A59F835D}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1102,7 +1120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K29" authorId="10" shapeId="0" xr:uid="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
+    <comment ref="K29" authorId="12" shapeId="0" xr:uid="{6BB9AE87-0F22-411C-94A5-B4B47AF58BA0}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1287,7 +1305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M31" authorId="11" shapeId="0" xr:uid="{A2079DE1-B458-45FD-A842-91298A20C566}">
+    <comment ref="M31" authorId="13" shapeId="0" xr:uid="{A2079DE1-B458-45FD-A842-91298A20C566}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1535,7 +1553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I35" authorId="12" shapeId="0" xr:uid="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
+    <comment ref="I35" authorId="14" shapeId="0" xr:uid="{B9CEBE49-3741-4E78-8050-25C8104DC552}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1850,7 +1868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G40" authorId="13" shapeId="0" xr:uid="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
+    <comment ref="G40" authorId="15" shapeId="0" xr:uid="{BC093F33-8C49-409A-B6B7-FD37F4A75DA3}">
       <text>
         <t xml:space="preserve">[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -1889,7 +1907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E43" authorId="14" shapeId="0" xr:uid="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
+    <comment ref="E43" authorId="16" shapeId="0" xr:uid="{6A673571-45B8-49C0-9F22-B54C0EA24752}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2017,7 +2035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K44" authorId="15" shapeId="0" xr:uid="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
+    <comment ref="K44" authorId="17" shapeId="0" xr:uid="{9DA15C1C-2ADF-486D-83D7-CF3E247B5DE8}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2025,7 +2043,7 @@
     전송을 통해 hci 추적 데이터를 보내는 함수</t>
       </text>
     </comment>
-    <comment ref="I47" authorId="16" shapeId="0" xr:uid="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
+    <comment ref="I47" authorId="18" shapeId="0" xr:uid="{65C98438-9758-4D35-BF7D-F62EAD43CA7C}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2101,7 +2119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K51" authorId="17" shapeId="0" xr:uid="{6EA8C629-9993-46C6-A087-93837636CB40}">
+    <comment ref="K51" authorId="19" shapeId="0" xr:uid="{6EA8C629-9993-46C6-A087-93837636CB40}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2109,7 +2127,7 @@
     가능한 많은 데이터를 보내는 테스트 함수</t>
       </text>
     </comment>
-    <comment ref="M51" authorId="18" shapeId="0" xr:uid="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
+    <comment ref="M51" authorId="20" shapeId="0" xr:uid="{62D68D75-ACD8-4EC1-B15A-164C348E6BF2}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2117,7 +2135,7 @@
     가능한 많은 데이터를 보내는 테스트 함수</t>
       </text>
     </comment>
-    <comment ref="M52" authorId="19" shapeId="0" xr:uid="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
+    <comment ref="M52" authorId="21" shapeId="0" xr:uid="{1B10A8DB-4982-4A0F-BF0B-278E4E81D02F}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2126,7 +2144,7 @@
 없으면 False</t>
       </text>
     </comment>
-    <comment ref="I59" authorId="20" shapeId="0" xr:uid="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
+    <comment ref="I59" authorId="22" shapeId="0" xr:uid="{EB3E1A67-2A20-48B4-A096-A5C983FFDD3E}">
       <text>
         <t xml:space="preserve">[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -2137,7 +2155,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="K61" authorId="21" shapeId="0" xr:uid="{97AD7065-CF38-4472-BC49-676025D10EB8}">
+    <comment ref="K61" authorId="23" shapeId="0" xr:uid="{97AD7065-CF38-4472-BC49-676025D10EB8}">
       <text>
         <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -3574,7 +3592,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3647,6 +3665,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -4047,9 +4071,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -4149,9 +4170,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -4182,7 +4200,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1">
@@ -4215,7 +4233,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1">
@@ -4257,7 +4275,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1">
@@ -4269,6 +4287,9 @@
     <xf numFmtId="0" fontId="17" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4278,7 +4299,10 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4832,6 +4856,12 @@
   <threadedComment ref="O15" dT="2022-11-30T06:55:20.40" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{C9FB7DAD-5DDC-4399-8A44-DEF628271C75}">
     <text>성공하면 1을 반환하고, 입력 매개 변수가 범위를 벗어나면 0xFF를 반환합니다.</text>
   </threadedComment>
+  <threadedComment ref="K16" dT="2022-12-15T02:26:27.87" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{B44307AE-C7C2-42B1-B54E-E1BA9BFD21B7}">
+    <text>Check to see if there is any data ready in the RX FIFO.</text>
+  </threadedComment>
+  <threadedComment ref="K17" dT="2022-12-15T02:25:40.58" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{FCC7E135-E087-4D67-9EA3-671A48F4D91D}">
+    <text>Read one byte via the RX line.</text>
+  </threadedComment>
   <threadedComment ref="K18" dT="2022-11-23T06:47:06.81" personId="{F2E6BAF2-849A-47D3-983F-1A394E5FC3BC}" id="{C78B3C0A-6A2B-411F-BC5C-56658A712951}">
     <text>바이트 집합을 순차적으로 쓰는 함수</text>
   </threadedComment>
@@ -4906,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CD9804-2490-4F6A-966A-5BB5914DA299}">
   <dimension ref="B2:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M54" sqref="M54"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4931,125 +4961,125 @@
   <sheetData>
     <row r="2" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
     </row>
     <row r="4" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="57">
         <v>1</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="58" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="57">
         <v>1</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="M5" s="75" t="s">
+      <c r="M5" s="73" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="73">
+      <c r="H6" s="71">
         <v>1</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="27" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="73">
+      <c r="H7" s="71">
         <v>1</v>
       </c>
-      <c r="I7" s="74" t="s">
+      <c r="I7" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="28" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="62">
+      <c r="H8" s="60">
         <v>1</v>
       </c>
-      <c r="I8" s="63" t="s">
+      <c r="I8" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="68.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="69" t="s">
         <v>283</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="26" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>285</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="O10" s="75" t="s">
+      <c r="O10" s="73" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="O11" s="29" t="s">
+      <c r="M11" s="27"/>
+      <c r="O11" s="28" t="s">
         <v>258</v>
       </c>
     </row>
@@ -5057,261 +5087,246 @@
       <c r="C12" t="s">
         <v>284</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="54" t="s">
+      <c r="G12" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="27" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="I13" s="32" t="s">
+      <c r="I13" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="M13" s="29"/>
-      <c r="O13" s="75" t="s">
+      <c r="M13" s="28"/>
+      <c r="O13" s="73" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="I14" s="28" t="s">
+      <c r="G14" s="27"/>
+      <c r="I14" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="O14" s="28" t="s">
+      <c r="O14" s="27" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="I15" s="35" t="s">
+      <c r="G15" s="27"/>
+      <c r="I15" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="O15" s="28" t="s">
+      <c r="O15" s="27" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="I16" s="28" t="s">
+      <c r="G16" s="27"/>
+      <c r="I16" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="O16" s="28"/>
-    </row>
-    <row r="17" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C17" s="3"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="28" t="s">
+      <c r="O16" s="27"/>
+    </row>
+    <row r="17" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D17" s="35"/>
+      <c r="E17" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="I17" s="29" t="s">
+      <c r="G17" s="27"/>
+      <c r="I17" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="O17" s="28" t="s">
+      <c r="O17" s="27" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="28" t="s">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.45">
+      <c r="D18" s="35"/>
+      <c r="E18" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="76" t="s">
+      <c r="G18" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="O18" s="28" t="s">
+      <c r="O18" s="27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="3"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="35" t="s">
+    <row r="19" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D19" s="35"/>
+      <c r="E19" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="76" t="s">
+      <c r="G19" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="K19" s="38" t="s">
+      <c r="K19" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="O19" s="29" t="s">
+      <c r="O19" s="28" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="3"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="35" t="s">
+    <row r="20" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D20" s="35"/>
+      <c r="E20" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="K20" s="39" t="s">
+      <c r="G20" s="27"/>
+      <c r="K20" s="37" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="3"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="29" t="s">
+    <row r="21" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D21" s="35"/>
+      <c r="E21" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="56" t="s">
+      <c r="G21" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="55" t="s">
+      <c r="I21" s="53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B22" s="3"/>
-      <c r="D22" s="37"/>
-      <c r="I22" s="27" t="s">
+    <row r="22" spans="3:15" x14ac:dyDescent="0.45">
+      <c r="D22" s="35"/>
+      <c r="I22" s="26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="3"/>
-      <c r="D23" s="37"/>
-      <c r="I23" s="28" t="s">
+    <row r="23" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D23" s="35"/>
+      <c r="I23" s="27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="3"/>
-      <c r="D24" s="36"/>
-      <c r="I24" s="28" t="s">
+    <row r="24" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D24" s="35"/>
+      <c r="I24" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="K24" s="32" t="s">
+      <c r="K24" s="31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="3"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="71" t="s">
+    <row r="25" spans="3:15" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D25" s="35"/>
+      <c r="E25" s="69" t="s">
         <v>253</v>
       </c>
-      <c r="I25" s="28"/>
-      <c r="K25" s="29" t="s">
+      <c r="I25" s="27"/>
+      <c r="K25" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B26" s="3"/>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>270</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="I26" s="28"/>
+      <c r="D26" s="35"/>
+      <c r="I26" s="27"/>
       <c r="J26" s="2"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="3"/>
-      <c r="D27" s="36"/>
-      <c r="I27" s="28" t="s">
+    </row>
+    <row r="27" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D27" s="35"/>
+      <c r="I27" s="27" t="s">
         <v>288</v>
       </c>
       <c r="J27" s="2"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="28" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C28" t="s">
         <v>271</v>
       </c>
-      <c r="G28" s="33" t="s">
+      <c r="G28" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="27" t="s">
         <v>289</v>
       </c>
       <c r="J28" s="2"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="29" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C29" t="s">
         <v>272</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="I29" s="57" t="s">
+      <c r="I29" s="55" t="s">
         <v>286</v>
       </c>
-      <c r="K29" s="32" t="s">
+      <c r="K29" s="31" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C30" t="s">
         <v>273</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="M30" s="31" t="s">
+      <c r="M30" s="30" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="3:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C31" t="s">
         <v>274</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="M31" s="29" t="s">
+      <c r="I31" s="27"/>
+      <c r="M31" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="O31" s="31" t="s">
+      <c r="O31" s="30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="G32" s="28" t="s">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.45">
+      <c r="G32" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="35"/>
-      <c r="O32" s="28" t="s">
+      <c r="I32" s="34"/>
+      <c r="O32" s="27" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5319,14 +5334,14 @@
       <c r="C33" t="s">
         <v>270</v>
       </c>
-      <c r="E33" s="43"/>
-      <c r="G33" s="28" t="s">
+      <c r="E33" s="41"/>
+      <c r="G33" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="O33" s="28" t="s">
+      <c r="O33" s="27" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5334,16 +5349,16 @@
       <c r="C34" t="s">
         <v>275</v>
       </c>
-      <c r="G34" s="29" t="s">
+      <c r="G34" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="O34" s="28" t="s">
+      <c r="O34" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="Q34" s="30" t="s">
+      <c r="Q34" s="29" t="s">
         <v>119</v>
       </c>
     </row>
@@ -5351,13 +5366,13 @@
       <c r="C35" t="s">
         <v>276</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="I35" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="O35" s="28" t="s">
+      <c r="O35" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="Q35" s="30" t="s">
+      <c r="Q35" s="29" t="s">
         <v>120</v>
       </c>
     </row>
@@ -5365,24 +5380,24 @@
       <c r="C36" t="s">
         <v>274</v>
       </c>
-      <c r="I36" s="28" t="s">
+      <c r="I36" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="O36" s="29" t="s">
+      <c r="O36" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="Q36" s="29" t="s">
+      <c r="Q36" s="28" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.45">
-      <c r="I37" s="28"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C38" t="s">
         <v>270</v>
       </c>
-      <c r="I38" s="42" t="s">
+      <c r="I38" s="40" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5390,13 +5405,13 @@
       <c r="C39" t="s">
         <v>277</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="I39" s="35" t="s">
+      <c r="I39" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="K39" s="32" t="s">
+      <c r="K39" s="31" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5404,13 +5419,13 @@
       <c r="C40" t="s">
         <v>278</v>
       </c>
-      <c r="G40" s="29" t="s">
+      <c r="G40" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="I40" s="34" t="s">
+      <c r="I40" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="29" t="s">
+      <c r="K40" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5418,13 +5433,13 @@
       <c r="C41" t="s">
         <v>274</v>
       </c>
-      <c r="I41" s="28"/>
+      <c r="I41" s="27"/>
     </row>
     <row r="42" spans="3:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I42" s="42" t="s">
+      <c r="I42" s="40" t="s">
         <v>128</v>
       </c>
     </row>
@@ -5432,16 +5447,16 @@
       <c r="C43" t="s">
         <v>270</v>
       </c>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="28" t="s">
+      <c r="I43" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="K43" s="32" t="s">
+      <c r="K43" s="31" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5449,11 +5464,11 @@
       <c r="C44" t="s">
         <v>279</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E44" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="I44" s="28"/>
-      <c r="K44" s="28" t="s">
+      <c r="I44" s="27"/>
+      <c r="K44" s="27" t="s">
         <v>83</v>
       </c>
     </row>
@@ -5461,19 +5476,19 @@
       <c r="C45" t="s">
         <v>280</v>
       </c>
-      <c r="I45" s="28"/>
-      <c r="K45" s="29"/>
+      <c r="I45" s="27"/>
+      <c r="K45" s="28"/>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C46" t="s">
         <v>274</v>
       </c>
-      <c r="I46" s="42" t="s">
+      <c r="I46" s="40" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.45">
-      <c r="I47" s="65" t="s">
+      <c r="I47" s="63" t="s">
         <v>125</v>
       </c>
     </row>
@@ -5481,7 +5496,7 @@
       <c r="C48" t="s">
         <v>270</v>
       </c>
-      <c r="I48" s="65" t="s">
+      <c r="I48" s="63" t="s">
         <v>208</v>
       </c>
     </row>
@@ -5492,10 +5507,10 @@
       <c r="G49" t="s">
         <v>122</v>
       </c>
-      <c r="I49" s="65" t="s">
+      <c r="I49" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="31" t="s">
         <v>131</v>
       </c>
     </row>
@@ -5506,8 +5521,8 @@
       <c r="G50" t="s">
         <v>121</v>
       </c>
-      <c r="I50" s="28"/>
-      <c r="K50" s="28" t="s">
+      <c r="I50" s="27"/>
+      <c r="K50" s="27" t="s">
         <v>132</v>
       </c>
     </row>
@@ -5515,31 +5530,31 @@
       <c r="C51" t="s">
         <v>274</v>
       </c>
-      <c r="I51" s="29" t="s">
+      <c r="I51" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="K51" s="80" t="s">
+      <c r="K51" s="75" t="s">
         <v>108</v>
       </c>
-      <c r="M51" s="55" t="s">
+      <c r="M51" s="53" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="M52" s="27" t="s">
+      <c r="M52" s="26" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="53" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="M53" s="28"/>
+      <c r="M53" s="27"/>
     </row>
     <row r="54" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="M54" s="29" t="s">
+      <c r="M54" s="28" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="55" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I55" s="55" t="s">
+      <c r="I55" s="53" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5547,47 +5562,47 @@
       <c r="G56" t="s">
         <v>216</v>
       </c>
-      <c r="I56" s="64" t="s">
+      <c r="I56" s="62" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="57" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I57" s="65" t="s">
+      <c r="I57" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="K57" s="32" t="s">
+      <c r="K57" s="31" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="58" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="I58" s="28"/>
-      <c r="K58" s="27" t="s">
+      <c r="I58" s="27"/>
+      <c r="K58" s="26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="59" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I59" s="66" t="s">
+      <c r="I59" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="K59" s="28" t="s">
+      <c r="K59" s="27" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="60" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="K60" s="28" t="s">
+      <c r="K60" s="80" t="s">
         <v>210</v>
       </c>
       <c r="M60" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="K61" s="65" t="s">
+    <row r="61" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K61" s="79" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="62" spans="3:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="K62" s="29"/>
+      <c r="K62" s="28"/>
     </row>
     <row r="63" spans="3:13" x14ac:dyDescent="0.45">
       <c r="I63" t="s">
@@ -5617,7 +5632,7 @@
     </row>
     <row r="68" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="69" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I69" s="55" t="s">
+      <c r="I69" s="53" t="s">
         <v>248</v>
       </c>
       <c r="M69" t="s">
@@ -5625,15 +5640,15 @@
       </c>
     </row>
     <row r="70" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I70" s="28" t="s">
+      <c r="I70" s="27" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="71" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I71" s="53" t="s">
+      <c r="I71" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="K71" s="70" t="s">
+      <c r="K71" s="68" t="s">
         <v>251</v>
       </c>
       <c r="M71" t="s">
@@ -5641,10 +5656,10 @@
       </c>
     </row>
     <row r="72" spans="9:13" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I72" s="29" t="s">
+      <c r="I72" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="K72" s="30" t="s">
+      <c r="K72" s="29" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5679,509 +5694,509 @@
   <sheetData>
     <row r="2" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="3" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="87" x14ac:dyDescent="0.45">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="2:6" ht="203" x14ac:dyDescent="0.45">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.45">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B9" s="22"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B10" s="22"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B16" s="22"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B17" s="22"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="16"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="2:6" ht="87" x14ac:dyDescent="0.45">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B21" s="22"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.45">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.45">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B26" s="22"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="16"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="16"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="2:6" ht="203" x14ac:dyDescent="0.45">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="16"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.45">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="16"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="16"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B31" s="22"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="16"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B32" s="22"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="16"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="16"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="2:6" ht="43.5" x14ac:dyDescent="0.45">
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="16"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="2:6" ht="145" x14ac:dyDescent="0.45">
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="2:6" ht="43.5" x14ac:dyDescent="0.45">
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B37" s="22"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.45">
-      <c r="B38" s="23"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14" t="s">
+      <c r="B38" s="22"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="16"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="16"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B41" s="22"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B42" s="23"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B43" s="22"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B44" s="22"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="16"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B45" s="22"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="16"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B46" s="22"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="16"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B47" s="22"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="16"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B48" s="22"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="15"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B49" s="22"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="16"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="15"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B50" s="22"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="15"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B51" s="22"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B52" s="22"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B53" s="22"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="16"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B54" s="4"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B55" s="4"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="15"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B56" s="4"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="16"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="15"/>
     </row>
     <row r="57" spans="2:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B57" s="5"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6201,1196 +6216,1196 @@
   <sheetData>
     <row r="1" spans="2:25" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="46"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="49"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="47"/>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="48"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="49"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="47"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="49"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="47"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="49"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="46"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="47"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="48"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
-      <c r="Y7" s="49"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="46"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="47"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="49"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="46"/>
+      <c r="Y8" s="47"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="48"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="49"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="47"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="49"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="46"/>
+      <c r="V10" s="46"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="46"/>
+      <c r="Y10" s="47"/>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="49"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="46"/>
+      <c r="V11" s="46"/>
+      <c r="W11" s="46"/>
+      <c r="X11" s="46"/>
+      <c r="Y11" s="47"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="49"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="47"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="49"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="46"/>
+      <c r="V13" s="46"/>
+      <c r="W13" s="46"/>
+      <c r="X13" s="46"/>
+      <c r="Y13" s="47"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="49"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="46"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="46"/>
+      <c r="V14" s="46"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="46"/>
+      <c r="Y14" s="47"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="49"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="47"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="49"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="47"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="45" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="49"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="47"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="49"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="46"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="47"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="45" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-      <c r="Y19" s="49"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="46"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="46"/>
+      <c r="Y19" s="47"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="48"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-      <c r="Y20" s="49"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="47"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="49"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="46"/>
+      <c r="U21" s="46"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="46"/>
+      <c r="Y21" s="47"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B22" s="47"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="48"/>
-      <c r="O22" s="48"/>
-      <c r="P22" s="48"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="48"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="48"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
-      <c r="X22" s="48"/>
-      <c r="Y22" s="49"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="46"/>
+      <c r="U22" s="46"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="47"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="48"/>
-      <c r="O23" s="48"/>
-      <c r="P23" s="48"/>
-      <c r="Q23" s="48"/>
-      <c r="R23" s="48"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="48"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="49"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="47"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="49"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="47"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="48"/>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
-      <c r="R25" s="48"/>
-      <c r="S25" s="48"/>
-      <c r="T25" s="48"/>
-      <c r="U25" s="48"/>
-      <c r="V25" s="48"/>
-      <c r="W25" s="48"/>
-      <c r="X25" s="48"/>
-      <c r="Y25" s="49"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="47"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="48"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="48"/>
-      <c r="U26" s="48"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="48"/>
-      <c r="X26" s="48"/>
-      <c r="Y26" s="49"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="47"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="48"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="48"/>
-      <c r="O27" s="48"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="48"/>
-      <c r="T27" s="48"/>
-      <c r="U27" s="48"/>
-      <c r="V27" s="48"/>
-      <c r="W27" s="48"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="49"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
+      <c r="Y27" s="47"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="48"/>
-      <c r="U28" s="48"/>
-      <c r="V28" s="48"/>
-      <c r="W28" s="48"/>
-      <c r="X28" s="48"/>
-      <c r="Y28" s="49"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="46"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="47"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
-      <c r="S29" s="48"/>
-      <c r="T29" s="48"/>
-      <c r="U29" s="48"/>
-      <c r="V29" s="48"/>
-      <c r="W29" s="48"/>
-      <c r="X29" s="48"/>
-      <c r="Y29" s="49"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
+      <c r="V29" s="46"/>
+      <c r="W29" s="46"/>
+      <c r="X29" s="46"/>
+      <c r="Y29" s="47"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B30" s="47"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="48"/>
-      <c r="O30" s="48"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="48"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="49"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="46"/>
+      <c r="V30" s="46"/>
+      <c r="W30" s="46"/>
+      <c r="X30" s="46"/>
+      <c r="Y30" s="47"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
-      <c r="O31" s="48"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-      <c r="S31" s="48"/>
-      <c r="T31" s="48"/>
-      <c r="U31" s="48"/>
-      <c r="V31" s="48"/>
-      <c r="W31" s="48"/>
-      <c r="X31" s="48"/>
-      <c r="Y31" s="49"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+      <c r="T31" s="46"/>
+      <c r="U31" s="46"/>
+      <c r="V31" s="46"/>
+      <c r="W31" s="46"/>
+      <c r="X31" s="46"/>
+      <c r="Y31" s="47"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-      <c r="R32" s="48"/>
-      <c r="S32" s="48"/>
-      <c r="T32" s="48"/>
-      <c r="U32" s="48"/>
-      <c r="V32" s="48"/>
-      <c r="W32" s="48"/>
-      <c r="X32" s="48"/>
-      <c r="Y32" s="49"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
+      <c r="V32" s="46"/>
+      <c r="W32" s="46"/>
+      <c r="X32" s="46"/>
+      <c r="Y32" s="47"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B33" s="47"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="48"/>
-      <c r="M33" s="48"/>
-      <c r="N33" s="48"/>
-      <c r="O33" s="48"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-      <c r="S33" s="48"/>
-      <c r="T33" s="48"/>
-      <c r="U33" s="48"/>
-      <c r="V33" s="48"/>
-      <c r="W33" s="48"/>
-      <c r="X33" s="48"/>
-      <c r="Y33" s="49"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="X33" s="46"/>
+      <c r="Y33" s="47"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="48"/>
-      <c r="S34" s="48"/>
-      <c r="T34" s="48"/>
-      <c r="U34" s="48"/>
-      <c r="V34" s="48"/>
-      <c r="W34" s="48"/>
-      <c r="X34" s="48"/>
-      <c r="Y34" s="49"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46"/>
+      <c r="R34" s="46"/>
+      <c r="S34" s="46"/>
+      <c r="T34" s="46"/>
+      <c r="U34" s="46"/>
+      <c r="V34" s="46"/>
+      <c r="W34" s="46"/>
+      <c r="X34" s="46"/>
+      <c r="Y34" s="47"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="48"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-      <c r="R35" s="48"/>
-      <c r="S35" s="48"/>
-      <c r="T35" s="48"/>
-      <c r="U35" s="48"/>
-      <c r="V35" s="48"/>
-      <c r="W35" s="48"/>
-      <c r="X35" s="48"/>
-      <c r="Y35" s="49"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="46"/>
+      <c r="S35" s="46"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="47"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="48"/>
-      <c r="V36" s="48"/>
-      <c r="W36" s="48"/>
-      <c r="X36" s="48"/>
-      <c r="Y36" s="49"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="46"/>
+      <c r="T36" s="46"/>
+      <c r="U36" s="46"/>
+      <c r="V36" s="46"/>
+      <c r="W36" s="46"/>
+      <c r="X36" s="46"/>
+      <c r="Y36" s="47"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="48"/>
-      <c r="M37" s="48"/>
-      <c r="N37" s="48"/>
-      <c r="O37" s="48"/>
-      <c r="P37" s="48"/>
-      <c r="Q37" s="48"/>
-      <c r="R37" s="48"/>
-      <c r="S37" s="48"/>
-      <c r="T37" s="48"/>
-      <c r="U37" s="48"/>
-      <c r="V37" s="48"/>
-      <c r="W37" s="48"/>
-      <c r="X37" s="48"/>
-      <c r="Y37" s="49"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="46"/>
+      <c r="V37" s="46"/>
+      <c r="W37" s="46"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="47"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B38" s="47"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="48"/>
-      <c r="T38" s="48"/>
-      <c r="U38" s="48"/>
-      <c r="V38" s="48"/>
-      <c r="W38" s="48"/>
-      <c r="X38" s="48"/>
-      <c r="Y38" s="49"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
+      <c r="T38" s="46"/>
+      <c r="U38" s="46"/>
+      <c r="V38" s="46"/>
+      <c r="W38" s="46"/>
+      <c r="X38" s="46"/>
+      <c r="Y38" s="47"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="48"/>
-      <c r="M39" s="48"/>
-      <c r="N39" s="48"/>
-      <c r="O39" s="48"/>
-      <c r="P39" s="48"/>
-      <c r="Q39" s="48"/>
-      <c r="R39" s="48"/>
-      <c r="S39" s="48"/>
-      <c r="T39" s="48"/>
-      <c r="U39" s="48"/>
-      <c r="V39" s="48"/>
-      <c r="W39" s="48"/>
-      <c r="X39" s="48"/>
-      <c r="Y39" s="49"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="46"/>
+      <c r="S39" s="46"/>
+      <c r="T39" s="46"/>
+      <c r="U39" s="46"/>
+      <c r="V39" s="46"/>
+      <c r="W39" s="46"/>
+      <c r="X39" s="46"/>
+      <c r="Y39" s="47"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="48"/>
-      <c r="O40" s="48"/>
-      <c r="P40" s="48"/>
-      <c r="Q40" s="48"/>
-      <c r="R40" s="48"/>
-      <c r="S40" s="48"/>
-      <c r="T40" s="48"/>
-      <c r="U40" s="48"/>
-      <c r="V40" s="48"/>
-      <c r="W40" s="48"/>
-      <c r="X40" s="48"/>
-      <c r="Y40" s="49"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="46"/>
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="46"/>
+      <c r="S40" s="46"/>
+      <c r="T40" s="46"/>
+      <c r="U40" s="46"/>
+      <c r="V40" s="46"/>
+      <c r="W40" s="46"/>
+      <c r="X40" s="46"/>
+      <c r="Y40" s="47"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="45" t="s">
         <v>203</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
-      <c r="O41" s="48"/>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
-      <c r="R41" s="48"/>
-      <c r="S41" s="48"/>
-      <c r="T41" s="48"/>
-      <c r="U41" s="48"/>
-      <c r="V41" s="48"/>
-      <c r="W41" s="48"/>
-      <c r="X41" s="48"/>
-      <c r="Y41" s="49"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="46"/>
+      <c r="N41" s="46"/>
+      <c r="O41" s="46"/>
+      <c r="P41" s="46"/>
+      <c r="Q41" s="46"/>
+      <c r="R41" s="46"/>
+      <c r="S41" s="46"/>
+      <c r="T41" s="46"/>
+      <c r="U41" s="46"/>
+      <c r="V41" s="46"/>
+      <c r="W41" s="46"/>
+      <c r="X41" s="46"/>
+      <c r="Y41" s="47"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="48"/>
-      <c r="V42" s="48"/>
-      <c r="W42" s="48"/>
-      <c r="X42" s="48"/>
-      <c r="Y42" s="49"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="46"/>
+      <c r="Q42" s="46"/>
+      <c r="R42" s="46"/>
+      <c r="S42" s="46"/>
+      <c r="T42" s="46"/>
+      <c r="U42" s="46"/>
+      <c r="V42" s="46"/>
+      <c r="W42" s="46"/>
+      <c r="X42" s="46"/>
+      <c r="Y42" s="47"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.45">
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="48"/>
-      <c r="X43" s="48"/>
-      <c r="Y43" s="49"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="46"/>
+      <c r="T43" s="46"/>
+      <c r="U43" s="46"/>
+      <c r="V43" s="46"/>
+      <c r="W43" s="46"/>
+      <c r="X43" s="46"/>
+      <c r="Y43" s="47"/>
     </row>
     <row r="44" spans="2:25" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="51"/>
-      <c r="T44" s="51"/>
-      <c r="U44" s="51"/>
-      <c r="V44" s="51"/>
-      <c r="W44" s="51"/>
-      <c r="X44" s="51"/>
-      <c r="Y44" s="52"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="49"/>
+      <c r="U44" s="49"/>
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -7415,391 +7430,391 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L3" s="68" t="s">
+      <c r="L3" s="66" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="L4" s="68" t="s">
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="L4" s="66" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="L5" s="68" t="s">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="L5" s="66" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="L6" s="68" t="s">
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="L6" s="66" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="L7" s="68" t="s">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="L7" s="66" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="L8" s="68" t="s">
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="L8" s="66" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="L9" s="68" t="s">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="L9" s="66" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="L10" s="68"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="L10" s="66"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="L11" s="68" t="s">
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="L11" s="66" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="L12" s="68" t="s">
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="L12" s="66" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="L13" s="68" t="s">
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="L13" s="66" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="L14" s="68" t="s">
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="66" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="L15" s="68"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="L15" s="66"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="L16" s="68" t="s">
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="L16" s="66" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="65" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="L17" s="68" t="s">
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="L17" s="66" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="L18" s="68"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="L18" s="66"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="L19" s="68" t="s">
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="L19" s="66" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B20" s="67" t="s">
+      <c r="B20" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="L20" s="68" t="s">
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="L20" s="66" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="L21" s="68"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="L21" s="66"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="65" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="L22" s="68" t="s">
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="L22" s="66" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="L23" s="68" t="s">
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="L23" s="66" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="L24" s="68"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="L24" s="66"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="L25" s="68" t="s">
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="L25" s="66" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L26" s="68" t="s">
+      <c r="L26" s="66" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L27" s="68"/>
+      <c r="L27" s="66"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L28" s="68" t="s">
+      <c r="L28" s="66" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L29" s="68" t="s">
+      <c r="L29" s="66" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L30" s="68"/>
+      <c r="L30" s="66"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L31" s="68" t="s">
+      <c r="L31" s="66" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="L32" s="68" t="s">
+      <c r="L32" s="66" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.45">
-      <c r="L33" s="68" t="s">
+      <c r="L33" s="66" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="34" spans="12:12" x14ac:dyDescent="0.45">
-      <c r="L34" s="68" t="s">
+      <c r="L34" s="66" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="35" spans="12:12" x14ac:dyDescent="0.45">
-      <c r="L35" s="68" t="s">
+      <c r="L35" s="66" t="s">
         <v>247</v>
       </c>
     </row>
@@ -7823,135 +7838,135 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="66" t="s">
         <v>151</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="66" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B5" s="68"/>
+      <c r="B5" s="66"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="66" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="67" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B8" s="68">
+      <c r="B8" s="66">
         <v>633</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="66" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="68"/>
+      <c r="B10" s="66"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="66" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="66" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="66" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="66" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B16" s="68"/>
+      <c r="B16" s="66"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="68"/>
+      <c r="B17" s="66"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="66" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="66" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="66" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="68"/>
+      <c r="B21" s="66"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B22" s="68"/>
+      <c r="B22" s="66"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B23" s="68"/>
+      <c r="B23" s="66"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="66" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="66" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B26" s="68"/>
+      <c r="B26" s="66"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B27" s="68"/>
+      <c r="B27" s="66"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="66" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="66" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="66" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="66" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="66" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>